<commit_message>
Initialized Flutter and Installed Dependencies and also done with setting up of database by creating tables
</commit_message>
<xml_diff>
--- a/Scoring.xlsx
+++ b/Scoring.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yashvit/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a5e7fedf47046736/Documents/Desktop/Final Year Project/Final_Year_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070DA7DF-976D-7445-8A0E-AFD1B85EBFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41740" windowHeight="23820" tabRatio="383" activeTab="3" xr2:uid="{9F55D3C2-66E2-4CF1-9355-923C688C1CB1}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="383" firstSheet="3" activeTab="3" xr2:uid="{9F55D3C2-66E2-4CF1-9355-923C688C1CB1}"/>
   </bookViews>
   <sheets>
     <sheet name="Participants" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -620,9 +619,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -660,7 +659,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -766,7 +765,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -908,7 +907,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -918,16 +917,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2157894A-B96A-400C-8B43-7087E673832E}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView zoomScale="121" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="16.6640625" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
@@ -941,7 +940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>101</v>
       </c>
@@ -955,7 +954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>103</v>
       </c>
@@ -969,7 +968,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>104</v>
       </c>
@@ -983,7 +982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>106</v>
       </c>
@@ -997,7 +996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>107</v>
       </c>
@@ -1011,7 +1010,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>108</v>
       </c>
@@ -1025,7 +1024,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>114</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>116</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>117</v>
       </c>
@@ -1067,7 +1066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>118</v>
       </c>
@@ -1081,7 +1080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>119</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>123</v>
       </c>
@@ -1138,31 +1137,31 @@
   </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="174" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O22" sqref="O22"/>
+      <selection pane="bottomRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="22.1640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="0.1640625" style="10" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="11" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="12" customWidth="1"/>
-    <col min="6" max="7" width="10.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="13" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5" style="12" customWidth="1"/>
-    <col min="11" max="12" width="10.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5" style="13" customWidth="1"/>
-    <col min="14" max="14" width="10.5" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.1640625" style="14"/>
+    <col min="1" max="1" width="5.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="22.109375" style="10" customWidth="1"/>
+    <col min="3" max="3" width="0.109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="8.44140625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="12" customWidth="1"/>
+    <col min="6" max="7" width="10.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="10.44140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" style="12" customWidth="1"/>
+    <col min="11" max="12" width="10.44140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="10.44140625" style="13" customWidth="1"/>
+    <col min="14" max="14" width="10.44140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="6" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="6" customFormat="1" ht="55.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -1212,7 +1211,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>117</v>
       </c>
@@ -1273,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>107</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9">
         <v>104</v>
       </c>
@@ -1395,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>103</v>
       </c>
@@ -1456,7 +1455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9">
         <v>106</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>114</v>
       </c>
@@ -1578,7 +1577,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9">
         <v>123</v>
       </c>
@@ -1639,7 +1638,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9">
         <v>119</v>
       </c>
@@ -1700,7 +1699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9">
         <v>101</v>
       </c>
@@ -1761,7 +1760,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9">
         <v>118</v>
       </c>
@@ -1822,7 +1821,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
         <v>108</v>
       </c>
@@ -1883,7 +1882,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="25.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="25.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
         <v>116</v>
       </c>
@@ -1974,17 +1973,17 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="5" width="9.83203125" style="3" customWidth="1"/>
+    <col min="4" max="5" width="9.77734375" style="3" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="7" max="7" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>117</v>
@@ -2037,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>107</v>
@@ -2067,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>104</v>
@@ -2097,7 +2096,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>103</v>
@@ -2127,7 +2126,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>106</v>
@@ -2157,7 +2156,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>114</v>
@@ -2187,7 +2186,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>123</v>
@@ -2217,7 +2216,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>119</v>
@@ -2247,7 +2246,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>101</v>
@@ -2277,7 +2276,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>118</v>
@@ -2307,7 +2306,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>108</v>
@@ -2337,7 +2336,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <f>IF(ISBLANK(Table25[[#This Row],[No]]),"", Table25[[#This Row],[No]])</f>
         <v>116</v>
@@ -2379,16 +2378,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2138F68-A4E4-476C-8AFD-B34EF90B5D34}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="97" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2399,7 +2398,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +2420,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2443,7 +2442,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2454,7 +2453,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>6</v>
       </c>
@@ -2462,7 +2461,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>7</v>
       </c>
@@ -2470,7 +2469,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>8</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>9</v>
       </c>
@@ -2486,7 +2485,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>10</v>
       </c>
@@ -2494,7 +2493,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>11</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>12</v>
       </c>
@@ -2510,7 +2509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>13</v>
       </c>
@@ -2518,7 +2517,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>14</v>
       </c>
@@ -2526,7 +2525,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>15</v>
       </c>
@@ -2534,7 +2533,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>16</v>
       </c>
@@ -2542,7 +2541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>17</v>
       </c>
@@ -2550,7 +2549,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>18</v>
       </c>
@@ -2558,7 +2557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>19</v>
       </c>
@@ -2566,7 +2565,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>20</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>21</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>22</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>23</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>24</v>
       </c>
@@ -2606,7 +2605,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>25</v>
       </c>
@@ -2614,7 +2613,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27">
         <v>26</v>
       </c>
@@ -2622,7 +2621,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>27</v>
       </c>
@@ -2630,7 +2629,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>28</v>
       </c>
@@ -2638,7 +2637,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>29</v>
       </c>
@@ -2646,7 +2645,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>30</v>
       </c>

</xml_diff>